<commit_message>
Correción de tablas a partir de últimas corridas
</commit_message>
<xml_diff>
--- a/Graficos B4.xlsx
+++ b/Graficos B4.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="150" windowWidth="12915" windowHeight="7500"/>
@@ -11,12 +11,12 @@
     <sheet name="GRAFICO 1" sheetId="2" r:id="rId2"/>
     <sheet name="GRAFICO 2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>ALGORITMO</t>
   </si>
@@ -31,24 +31,6 @@
   </si>
   <si>
     <t>TIEMPO (ns)</t>
-  </si>
-  <si>
-    <t>0.0628319</t>
-  </si>
-  <si>
-    <t>0.00628319</t>
-  </si>
-  <si>
-    <t>0.000628319</t>
-  </si>
-  <si>
-    <t>-0.0351377</t>
-  </si>
-  <si>
-    <t>-0.00332302</t>
-  </si>
-  <si>
-    <t>-0.000330389</t>
   </si>
 </sst>
 </file>
@@ -541,11 +523,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -637,7 +617,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> real relativo VS k</a:t>
+              <a:t> Real Relativo vs. K 	[1]</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -667,89 +647,78 @@
             </c:strRef>
           </c:tx>
           <c:xVal>
-            <c:strRef>
-              <c:f>DATOS!$C$2:$C$13</c:f>
-              <c:strCache>
-                <c:ptCount val="12"/>
+            <c:numRef>
+              <c:f>DATOS!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.0628319</c:v>
+                  <c:v>6.2799999999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.00628319</c:v>
+                  <c:v>6.28E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.000628319</c:v>
+                  <c:v>6.2799999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6,28E+00</c:v>
+                  <c:v>6.2799999999999995E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6,28E-01</c:v>
+                  <c:v>6.28E-6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6,28E-02</c:v>
+                  <c:v>6.2799999999999996E-7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6,28E-03</c:v>
+                  <c:v>6.2800000000000006E-8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6,28E-04</c:v>
+                  <c:v>6.2799999999999998E-9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6,28E-05</c:v>
+                  <c:v>6.28E-10</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6,28E-06</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6,28E-07</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>6,28E-08</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>6.2800000000000005E-11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>DATOS!$D$2:$D$13</c:f>
+              <c:f>DATOS!$D$2:$D$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>-3.5099999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-3.32E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3.3E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-3.2499999999999997E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-3.4000000000000001E-6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-4.1699999999999999E-7</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="7" formatCode="General">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="8" formatCode="General">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="0.00E+00">
-                  <c:v>-3.25</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="0.00E+00">
-                  <c:v>-0.34</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="0.00E+00">
-                  <c:v>-4.1700000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="9" formatCode="General">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -765,11 +734,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="125331712"/>
-        <c:axId val="125333888"/>
+        <c:axId val="169136640"/>
+        <c:axId val="169137216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="125331712"/>
+        <c:axId val="169136640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -779,23 +748,23 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125333888"/>
+        <c:crossAx val="169137216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="125333888"/>
+        <c:axId val="169137216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125331712"/>
+        <c:crossAx val="169136640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -841,17 +810,17 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> de corrida</a:t>
+              <a:t> de Corrida</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t> VS </a:t>
+              <a:t> vs. </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Pasos (N) </a:t>
+              <a:t>Pasos (N)	[2] </a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -884,7 +853,7 @@
             <c:numRef>
               <c:f>DATOS!$F$2:$F$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
@@ -898,29 +867,23 @@
                 <c:pt idx="3">
                   <c:v>100000</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="0.00E+00">
+                <c:pt idx="4">
                   <c:v>1000000</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="0.00E+00">
+                <c:pt idx="5">
                   <c:v>10000000</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="0.00E+00">
+                <c:pt idx="6">
                   <c:v>100000000</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="0.00E+00">
+                <c:pt idx="7">
                   <c:v>1000000000</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="0.00E+00">
+                <c:pt idx="8">
                   <c:v>10000000000</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="0.00E+00">
+                <c:pt idx="9">
                   <c:v>100000000000</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="0.00E+00">
-                  <c:v>1000000000000</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="0.00E+00">
-                  <c:v>10000000000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -941,31 +904,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>501700</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00E+00">
-                  <c:v>3010000000</c:v>
+                  <c:v>3500000</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0.00E+00">
-                  <c:v>3360000000000</c:v>
+                  <c:v>40000000</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00E+00">
-                  <c:v>30100000000000</c:v>
+                  <c:v>310000000</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="0.00E+00">
-                  <c:v>319000000000000</c:v>
+                  <c:v>3230000000</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0.00E+00">
-                  <c:v>3180000000000000</c:v>
+                  <c:v>32200000000</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00E+00">
-                  <c:v>3.08E+16</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="0.00E+00">
-                  <c:v>3.05E+17</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="0.00E+00">
-                  <c:v>3.05E+18</c:v>
+                  <c:v>320000000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -980,11 +937,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="125963264"/>
-        <c:axId val="125978496"/>
+        <c:axId val="169138944"/>
+        <c:axId val="169139520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="125963264"/>
+        <c:axId val="169138944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -992,11 +949,11 @@
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:minorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125978496"/>
+        <c:crossAx val="169139520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -1004,7 +961,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="125978496"/>
+        <c:axId val="169139520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1016,7 +973,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125963264"/>
+        <c:crossAx val="169138944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1394,22 +1351,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1426,209 +1383,212 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="8">
+      <c r="C2" s="7">
+        <v>6.2799999999999995E-2</v>
+      </c>
+      <c r="D2" s="7">
+        <v>-3.5099999999999999E-2</v>
+      </c>
+      <c r="E2" s="6">
         <v>0</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="7">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="8">
+      <c r="C3" s="7">
+        <v>6.28E-3</v>
+      </c>
+      <c r="D3" s="7">
+        <v>-3.32E-3</v>
+      </c>
+      <c r="E3" s="6">
         <v>0</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="7">
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="8">
+      <c r="C4" s="7">
+        <v>6.2799999999999998E-4</v>
+      </c>
+      <c r="D4" s="7">
+        <v>-3.3E-4</v>
+      </c>
+      <c r="E4" s="6">
         <v>0</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="7">
         <v>10000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="C5" s="5">
-        <v>6.28</v>
-      </c>
-      <c r="D5" s="7">
-        <v>-3.25</v>
-      </c>
-      <c r="E5" s="8">
-        <v>501700</v>
-      </c>
-      <c r="F5" s="1">
+      <c r="C5" s="3">
+        <v>6.2799999999999995E-5</v>
+      </c>
+      <c r="D5" s="5">
+        <v>-3.2499999999999997E-5</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7">
         <v>100000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>1</v>
       </c>
-      <c r="C6" s="5">
-        <v>0.628</v>
-      </c>
-      <c r="D6" s="7">
-        <v>-0.34</v>
-      </c>
-      <c r="E6" s="9">
-        <v>3010000000</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="C6" s="3">
+        <v>6.28E-6</v>
+      </c>
+      <c r="D6" s="5">
+        <v>-3.4000000000000001E-6</v>
+      </c>
+      <c r="E6" s="7">
+        <v>3500000</v>
+      </c>
+      <c r="F6" s="1">
         <v>1000000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>1</v>
       </c>
-      <c r="C7" s="5">
-        <v>6.2799999999999995E-2</v>
-      </c>
-      <c r="D7" s="7">
-        <v>-4.1700000000000001E-2</v>
-      </c>
-      <c r="E7" s="9">
-        <v>3360000000000</v>
-      </c>
-      <c r="F7" s="2">
+      <c r="C7" s="7">
+        <v>6.2799999999999996E-7</v>
+      </c>
+      <c r="D7" s="5">
+        <v>-4.1699999999999999E-7</v>
+      </c>
+      <c r="E7" s="7">
+        <v>40000000</v>
+      </c>
+      <c r="F7" s="1">
         <v>10000000</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>1</v>
       </c>
-      <c r="C8" s="5">
-        <v>6.28E-3</v>
-      </c>
-      <c r="D8" s="6">
+      <c r="C8" s="7">
+        <v>6.2800000000000006E-8</v>
+      </c>
+      <c r="D8" s="4">
         <v>0</v>
       </c>
-      <c r="E8" s="9">
-        <v>30100000000000</v>
-      </c>
-      <c r="F8" s="2">
+      <c r="E8" s="7">
+        <v>310000000</v>
+      </c>
+      <c r="F8" s="1">
         <v>100000000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>1</v>
       </c>
-      <c r="C9" s="5">
-        <v>6.2799999999999998E-4</v>
-      </c>
-      <c r="D9" s="6">
+      <c r="C9" s="7">
+        <v>6.2799999999999998E-9</v>
+      </c>
+      <c r="D9" s="4">
         <v>0</v>
       </c>
-      <c r="E9" s="9">
-        <v>319000000000000</v>
-      </c>
-      <c r="F9" s="2">
+      <c r="E9" s="7">
+        <v>3230000000</v>
+      </c>
+      <c r="F9" s="1">
         <v>1000000000</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>1</v>
       </c>
-      <c r="C10" s="5">
-        <v>6.2799999999999995E-5</v>
-      </c>
-      <c r="D10" s="6">
+      <c r="C10" s="7">
+        <v>6.28E-10</v>
+      </c>
+      <c r="D10" s="4">
         <v>0</v>
       </c>
-      <c r="E10" s="9">
-        <v>3180000000000000</v>
-      </c>
-      <c r="F10" s="2">
+      <c r="E10" s="7">
+        <v>32200000000</v>
+      </c>
+      <c r="F10" s="1">
         <v>10000000000</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>1</v>
       </c>
-      <c r="C11" s="5">
-        <v>6.28E-6</v>
-      </c>
-      <c r="D11" s="6">
+      <c r="C11" s="7">
+        <v>6.2800000000000005E-11</v>
+      </c>
+      <c r="D11" s="4">
         <v>0</v>
       </c>
-      <c r="E11" s="9">
-        <v>3.08E+16</v>
-      </c>
-      <c r="F11" s="2">
+      <c r="E11" s="7">
+        <v>320000000000</v>
+      </c>
+      <c r="F11" s="1">
         <v>100000000000</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>1</v>
-      </c>
-      <c r="C12" s="5">
-        <v>6.2799999999999996E-7</v>
-      </c>
-      <c r="D12" s="6">
-        <v>0</v>
-      </c>
-      <c r="E12" s="9">
-        <v>3.05E+17</v>
-      </c>
-      <c r="F12" s="2">
-        <v>1000000000000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>1</v>
-      </c>
-      <c r="C13" s="5">
-        <v>6.2800000000000006E-8</v>
-      </c>
-      <c r="D13" s="6">
-        <v>0</v>
-      </c>
-      <c r="E13" s="9">
-        <v>3.05E+18</v>
-      </c>
-      <c r="F13" s="2">
-        <v>10000000000000</v>
-      </c>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="7"/>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G20" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1639,14 +1599,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="BJ29"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K48" sqref="K48"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="29" spans="62:62" x14ac:dyDescent="0.25">
-      <c r="BJ29" s="10"/>
+      <c r="BJ29" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1660,7 +1620,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T46" sqref="T46"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>